<commit_message>
Looked further into battery possibilities, added some additional datasheets
</commit_message>
<xml_diff>
--- a/Documentation/Battery Life Calculations.xlsx
+++ b/Documentation/Battery Life Calculations.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Basic Battery Life Calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="Look Up Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Battery Type</t>
   </si>
@@ -37,12 +38,6 @@
     <t>Idle</t>
   </si>
   <si>
-    <t>Transmit</t>
-  </si>
-  <si>
-    <t>Receive</t>
-  </si>
-  <si>
     <t>PIC16LF1823</t>
   </si>
   <si>
@@ -59,13 +54,157 @@
   </si>
   <si>
     <t>THEORETICAL</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Constraints:</t>
+  </si>
+  <si>
+    <t>Clock Frequency</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Typ/Nom</t>
+  </si>
+  <si>
+    <t>Nominal Specs</t>
+  </si>
+  <si>
+    <t>Operating Current</t>
+  </si>
+  <si>
+    <t>1.3uA</t>
+  </si>
+  <si>
+    <t>1sps, 11 bit temp &amp; humidity</t>
+  </si>
+  <si>
+    <t>Sleep Current</t>
+  </si>
+  <si>
+    <t>Per MHz @ 1.8V</t>
+  </si>
+  <si>
+    <t>Operating Speed</t>
+  </si>
+  <si>
+    <t>Operating Current (Typ)</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Analog Voltage</t>
+  </si>
+  <si>
+    <t>Digital Voltage</t>
+  </si>
+  <si>
+    <t>ESP8266</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Ah</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>CR2032</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>DUTY CYCLE</t>
+  </si>
+  <si>
+    <t>Update Rate</t>
+  </si>
+  <si>
+    <t>Update Duration</t>
+  </si>
+  <si>
+    <t>per Minute</t>
+  </si>
+  <si>
+    <t>Update Current</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Transmit Current</t>
+  </si>
+  <si>
+    <t>Time in Sleep</t>
+  </si>
+  <si>
+    <t>Time in Transmit</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Nominal value from Energizer Spec</t>
+  </si>
+  <si>
+    <t>Based on 100mA drain in Energizer spec down to 0.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +220,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,7 +246,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -178,11 +334,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -194,8 +380,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,30 +694,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q31"/>
+  <dimension ref="A2:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -531,15 +736,21 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -548,9 +759,15 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="6"/>
@@ -563,13 +780,33 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="P5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="11">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -578,12 +815,28 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="P6" s="5"/>
+      <c r="Q6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="14">
+        <v>10</v>
+      </c>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14">
+        <v>400</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -593,9 +846,23 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -606,10 +873,15 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="7"/>
+      <c r="P8" s="5"/>
       <c r="Q8" s="11"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -620,77 +892,169 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
+      <c r="P9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="18"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="16">
+        <f>R28</f>
+        <v>2E-8</v>
+      </c>
+      <c r="D11" s="16">
+        <f>R24</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E11" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="16">
+        <f>SUM(C11:I11)</f>
+        <v>1.0120000000000001E-5</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="14">
+        <v>3</v>
+      </c>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="16">
+        <f t="shared" ref="J12:J13" si="0">SUM(C12:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="14">
+        <v>1.8</v>
+      </c>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="12">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="C13" s="16">
+        <v>1.2E-4</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1.3E-6</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.17</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="16">
+        <f t="shared" si="0"/>
+        <v>0.1701213</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="R13" s="16">
+        <v>0.12</v>
+      </c>
+      <c r="S13" s="16">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T13" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -701,11 +1065,15 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -716,9 +1084,15 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -729,9 +1103,15 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -742,9 +1122,15 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -755,9 +1141,15 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="10"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -769,10 +1161,19 @@
       <c r="K19" s="6"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -781,11 +1182,20 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="P20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -794,11 +1204,24 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="11">
+        <f>J13</f>
+        <v>0.1701213</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -807,9 +1230,17 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
+      <c r="P22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -820,9 +1251,21 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="S23" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="T23" s="14"/>
+      <c r="U23" s="17"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="22"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -833,37 +1276,81 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="16">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="17"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="D25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="D26" s="11">
+        <f>C6/J11</f>
+        <v>16106.719367588932</v>
+      </c>
+      <c r="E26" s="11">
+        <f>D26/24</f>
+        <v>671.11330698287213</v>
+      </c>
+      <c r="F26" s="11">
+        <f>E26/365</f>
+        <v>1.8386665944736222</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="7"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="7"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="11">
+        <f>C6/J13</f>
+        <v>0.95813986843505194</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -872,9 +1359,17 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
+      <c r="P27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -885,9 +1380,19 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="R28" s="16">
+        <v>2E-8</v>
+      </c>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="17"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="22"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -898,9 +1403,21 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R29" s="16">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="S29" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29" s="14"/>
+      <c r="U29" s="17"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="22"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -911,9 +1428,15 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="7"/>
-    </row>
-    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="8"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="17"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="23"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -924,6 +1447,206 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="10"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="R31" s="14">
+        <v>4</v>
+      </c>
+      <c r="S31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="T31" s="14"/>
+      <c r="U31" s="17"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P32" s="5"/>
+      <c r="Q32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="R32" s="16">
+        <f>R29*R31</f>
+        <v>1.2E-4</v>
+      </c>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="17"/>
+    </row>
+    <row r="33" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P33" s="5"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="7"/>
+    </row>
+    <row r="34" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="U34" s="7"/>
+    </row>
+    <row r="35" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P35" s="5"/>
+      <c r="Q35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="S35" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="T35" s="16">
+        <v>0.21</v>
+      </c>
+      <c r="U35" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P36" s="5"/>
+      <c r="Q36" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="R36" s="14"/>
+      <c r="S36" s="16">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="T36" s="14"/>
+      <c r="U36" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="16:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P37" s="8"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="14">
+        <v>3</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>